<commit_message>
Reworked all of the backend code to faciliate concurrecy and reworked front end to use the changed backend
</commit_message>
<xml_diff>
--- a/app/src/main/assets/Book.xlsx
+++ b/app/src/main/assets/Book.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22918"/>
   <workbookPr defaultThemeVersion="166925"/>
   <xr:revisionPtr revIDLastSave="442" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F8E40A43-5235-41A1-B759-66901D75D07E}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="2" firstSheet="1" windowHeight="8010" windowWidth="14805" xWindow="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="105"/>
   </bookViews>
   <sheets>
     <sheet name="Module" sheetId="1" r:id="rId1"/>
@@ -436,17 +436,42 @@
   <si>
     <t>PickUpDucks</t>
   </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Paypyrus</t>
+  </si>
+  <si>
+    <t>Tap anywhere to continue!</t>
+  </si>
+  <si>
+    <t>Get started with the basics</t>
+  </si>
+  <si>
+    <t>Starting out right ( to left!!!) with these preparatory lessons to get you going in the right (left) direction!</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -460,15 +485,25 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -788,14 +823,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
@@ -906,14 +940,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4601532C-3460-47AD-AB42-D440D6914B38}">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4601532C-3460-47AD-AB42-D440D6914B38}">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection pane="topLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -1047,14 +1080,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC0EBA9-A7F4-428C-BDF6-604F23BD7DE8}">
-  <dimension ref="A1:K29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC0EBA9-A7F4-428C-BDF6-604F23BD7DE8}">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection pane="topLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
@@ -1103,56 +1135,44 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" t="s">
-        <v>46</v>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0">
+        <v>2</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>0</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0">
+        <v>2</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1163,62 +1183,68 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" t="s">
-        <v>48</v>
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" t="s">
-        <v>52</v>
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1229,25 +1255,16 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1258,22 +1275,22 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="I8" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1284,22 +1301,25 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="I9" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1310,22 +1330,22 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="H10" t="s">
-        <v>69</v>
+        <v>60</v>
+      </c>
+      <c r="I10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1336,25 +1356,22 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="G11" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="I11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1365,22 +1382,22 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>66</v>
+      </c>
+      <c r="F12" t="s">
+        <v>67</v>
       </c>
       <c r="G12" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H12" t="s">
-        <v>77</v>
-      </c>
-      <c r="I12" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1388,25 +1405,28 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>70</v>
+      </c>
+      <c r="F13" t="s">
+        <v>71</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="H13" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="I13" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1414,22 +1434,25 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" t="s">
-        <v>84</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="G14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1440,19 +1463,22 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H15" t="s">
-        <v>87</v>
+        <v>81</v>
+      </c>
+      <c r="I15" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1463,22 +1489,19 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" t="s">
-        <v>89</v>
-      </c>
-      <c r="H16" t="s">
-        <v>90</v>
-      </c>
-      <c r="I16" t="s">
-        <v>91</v>
+        <v>83</v>
+      </c>
+      <c r="F16" t="s">
+        <v>84</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1489,13 +1512,19 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>85</v>
+      </c>
+      <c r="G17" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1506,19 +1535,22 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
-      </c>
-      <c r="F18" t="s">
-        <v>94</v>
-      </c>
-      <c r="J18">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="G18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1529,13 +1561,13 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D19">
-        <v>6</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1546,22 +1578,19 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" t="s">
-        <v>95</v>
-      </c>
-      <c r="H20" t="s">
-        <v>96</v>
-      </c>
-      <c r="I20" t="s">
-        <v>97</v>
+        <v>93</v>
+      </c>
+      <c r="F20" t="s">
+        <v>94</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1572,65 +1601,62 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D21">
-        <v>4</v>
-      </c>
-      <c r="E21" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" t="s">
-        <v>99</v>
-      </c>
-      <c r="J21">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" t="s">
-        <v>100</v>
+        <v>70</v>
+      </c>
+      <c r="G22" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" t="s">
+        <v>96</v>
+      </c>
+      <c r="I22" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>101</v>
-      </c>
-      <c r="G23" t="s">
-        <v>102</v>
-      </c>
-      <c r="H23" t="s">
-        <v>103</v>
-      </c>
-      <c r="I23" t="s">
-        <v>104</v>
+        <v>98</v>
+      </c>
+      <c r="F23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1641,25 +1667,16 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" t="s">
-        <v>105</v>
-      </c>
-      <c r="H24" t="s">
-        <v>106</v>
-      </c>
-      <c r="I24" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1670,22 +1687,22 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G25" t="s">
-        <v>109</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
+      </c>
+      <c r="H25" t="s">
+        <v>103</v>
       </c>
       <c r="I25" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1696,22 +1713,25 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>112</v>
+        <v>53</v>
+      </c>
+      <c r="F26" t="s">
+        <v>54</v>
       </c>
       <c r="G26" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H26" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="I26" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1722,22 +1742,22 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G27" t="s">
-        <v>117</v>
-      </c>
-      <c r="H27" t="s">
-        <v>118</v>
+        <v>109</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="I27" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1748,25 +1768,22 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="G28" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="H28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="I28" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1777,21 +1794,76 @@
         <v>0</v>
       </c>
       <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>116</v>
+      </c>
+      <c r="G29" t="s">
+        <v>117</v>
+      </c>
+      <c r="H29" t="s">
+        <v>118</v>
+      </c>
+      <c r="I29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" t="s">
+        <v>120</v>
+      </c>
+      <c r="H30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
         <v>7</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
         <v>75</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G31" t="s">
         <v>123</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H31" t="s">
         <v>124</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I31" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1801,14 +1873,13 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD447A5-A66D-423E-BEF4-4A4BB39A2411}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD447A5-A66D-423E-BEF4-4A4BB39A2411}">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
@@ -1876,14 +1947,13 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30587C1B-3062-4125-8D73-822059D87865}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30587C1B-3062-4125-8D73-822059D87865}">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection pane="topLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1918,14 +1988,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996951D6-D811-4EA7-B062-C55A0ACDC35A}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996951D6-D811-4EA7-B062-C55A0ACDC35A}">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Updated the destinations and nav graph to better match  the structure of the individual modules
</commit_message>
<xml_diff>
--- a/app/src/main/assets/Book.xlsx
+++ b/app/src/main/assets/Book.xlsx
@@ -455,7 +455,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" count="8" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
@@ -1083,7 +1083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC0EBA9-A7F4-428C-BDF6-604F23BD7DE8}">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="topLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1169,7 +1169,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>138</v>
+        <v>7</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>9</v>
@@ -1254,17 +1254,23 @@
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
+        <v>49</v>
+      </c>
+      <c r="G7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1274,23 +1280,26 @@
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1300,26 +1309,23 @@
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="0">
         <v>2</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1329,23 +1335,23 @@
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0">
         <v>3</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1355,23 +1361,23 @@
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="0">
         <v>4</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1381,23 +1387,26 @@
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="0">
         <v>5</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="I12" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1407,26 +1416,23 @@
       <c r="B13">
         <v>0</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="0">
         <v>6</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G13" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="I13" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1434,25 +1440,25 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H14" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I14" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1463,22 +1469,19 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" t="s">
-        <v>81</v>
-      </c>
-      <c r="I15" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="F15" t="s">
+        <v>84</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1489,19 +1492,19 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" t="s">
-        <v>84</v>
-      </c>
-      <c r="J16">
-        <v>1</v>
+        <v>85</v>
+      </c>
+      <c r="G16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1512,19 +1515,22 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G17" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H17" t="s">
-        <v>87</v>
+        <v>90</v>
+      </c>
+      <c r="I17" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1535,22 +1541,13 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" t="s">
-        <v>89</v>
-      </c>
-      <c r="H18" t="s">
-        <v>90</v>
-      </c>
-      <c r="I18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1561,13 +1558,19 @@
         <v>1</v>
       </c>
       <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
         <v>4</v>
       </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
       <c r="E19" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="F19" t="s">
+        <v>94</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1578,18 +1581,12 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D20">
-        <v>4</v>
-      </c>
-      <c r="E20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" t="s">
-        <v>94</v>
-      </c>
-      <c r="J20">
+        <v>6</v>
+      </c>
+      <c r="K20">
         <v>1</v>
       </c>
     </row>
@@ -1601,13 +1598,22 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D21">
-        <v>6</v>
-      </c>
-      <c r="K21">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" t="s">
+        <v>96</v>
+      </c>
+      <c r="I21" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1618,45 +1624,39 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" t="s">
-        <v>95</v>
-      </c>
-      <c r="H22" t="s">
-        <v>96</v>
-      </c>
-      <c r="I22" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="F22" t="s">
+        <v>99</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>99</v>
-      </c>
-      <c r="J23">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1667,16 +1667,22 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="G24" t="s">
+        <v>102</v>
+      </c>
+      <c r="H24" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1687,22 +1693,25 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>101</v>
+        <v>53</v>
+      </c>
+      <c r="F25" t="s">
+        <v>54</v>
       </c>
       <c r="G25" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H25" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I25" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1713,25 +1722,22 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="G26" t="s">
-        <v>105</v>
-      </c>
-      <c r="H26" t="s">
-        <v>106</v>
+        <v>109</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="I26" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1742,22 +1748,22 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G27" t="s">
-        <v>109</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
+      </c>
+      <c r="H27" t="s">
+        <v>114</v>
       </c>
       <c r="I27" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1768,22 +1774,22 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G28" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H28" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="I28" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1794,22 +1800,25 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>116</v>
+        <v>70</v>
+      </c>
+      <c r="F29" t="s">
+        <v>71</v>
       </c>
       <c r="G29" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H29" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="I29" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1820,50 +1829,21 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G30" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H30" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="I30" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31">
-        <v>2</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>7</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>75</v>
-      </c>
-      <c r="G31" t="s">
-        <v>123</v>
-      </c>
-      <c r="H31" t="s">
-        <v>124</v>
-      </c>
-      <c r="I31" t="s">
         <v>125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Switching over from using nav_graph to moving between fragments manually
</commit_message>
<xml_diff>
--- a/app/src/main/assets/Book.xlsx
+++ b/app/src/main/assets/Book.xlsx
@@ -450,6 +450,42 @@
   </si>
   <si>
     <t>Starting out right ( to left!!!) with these preparatory lessons to get you going in the right (left) direction!</t>
+  </si>
+  <si>
+    <t>Splash Screen</t>
+  </si>
+  <si>
+    <t>splash</t>
+  </si>
+  <si>
+    <t>moduleSelection</t>
+  </si>
+  <si>
+    <t>moduleContent</t>
+  </si>
+  <si>
+    <t>ModuleList</t>
+  </si>
+  <si>
+    <t>lessonSelection</t>
+  </si>
+  <si>
+    <t>moduleList</t>
+  </si>
+  <si>
+    <t>lessonContent</t>
+  </si>
+  <si>
+    <t>lessonImage</t>
+  </si>
+  <si>
+    <t>mediaPlayer</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>activity</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC0EBA9-A7F4-428C-BDF6-604F23BD7DE8}">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="topLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1146,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="0">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>136</v>
@@ -1166,7 +1202,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>7</v>
@@ -1175,30 +1211,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
+    <row r="4">
+      <c r="A4" s="0">
         <v>0</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="0">
+        <v>2</v>
+      </c>
+      <c r="D4" s="0">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" t="s">
-        <v>42</v>
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1209,22 +1239,22 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D5" s="0">
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1235,42 +1265,42 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D6" s="0">
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="0">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="0">
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" t="s">
-        <v>52</v>
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1281,25 +1311,22 @@
         <v>0</v>
       </c>
       <c r="C8" s="0">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="D8" s="0">
+        <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1310,22 +1337,25 @@
         <v>0</v>
       </c>
       <c r="C9" s="0">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="D9" s="0">
+        <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1336,22 +1366,22 @@
         <v>0</v>
       </c>
       <c r="C10" s="0">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D10" s="0">
+        <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1362,22 +1392,22 @@
         <v>0</v>
       </c>
       <c r="C11" s="0">
+        <v>3</v>
+      </c>
+      <c r="D11" s="0">
         <v>4</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
       <c r="E11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H11" t="s">
-        <v>69</v>
+        <v>64</v>
+      </c>
+      <c r="I11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1388,25 +1418,22 @@
         <v>0</v>
       </c>
       <c r="C12" s="0">
-        <v>5</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D12" s="0">
+        <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
-      </c>
-      <c r="I12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1417,22 +1444,25 @@
         <v>0</v>
       </c>
       <c r="C13" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>70</v>
+      </c>
+      <c r="F13" t="s">
+        <v>71</v>
       </c>
       <c r="G13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1440,25 +1470,25 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C14" s="0">
+        <v>6</v>
+      </c>
+      <c r="D14" s="0">
+        <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I14" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1469,19 +1499,22 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="D15" s="0">
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" t="s">
-        <v>84</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
+        <v>79</v>
+      </c>
+      <c r="G15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1492,19 +1525,19 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="D16" s="0">
+        <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
-      </c>
-      <c r="G16" t="s">
-        <v>86</v>
-      </c>
-      <c r="H16" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="F16" t="s">
+        <v>84</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1515,22 +1548,19 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D17" s="0">
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H17" t="s">
-        <v>90</v>
-      </c>
-      <c r="I17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1541,13 +1571,22 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>4</v>
-      </c>
-      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="D18" s="0">
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>92</v>
+        <v>88</v>
+      </c>
+      <c r="G18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1558,19 +1597,13 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>5</v>
-      </c>
-      <c r="D19">
         <v>4</v>
       </c>
+      <c r="D19" s="0">
+        <v>7</v>
+      </c>
       <c r="E19" t="s">
-        <v>93</v>
-      </c>
-      <c r="F19" t="s">
-        <v>94</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1581,12 +1614,18 @@
         <v>1</v>
       </c>
       <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" s="0">
         <v>6</v>
       </c>
-      <c r="D20">
-        <v>6</v>
-      </c>
-      <c r="K20">
+      <c r="E20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" t="s">
+        <v>94</v>
+      </c>
+      <c r="J20">
         <v>1</v>
       </c>
     </row>
@@ -1598,22 +1637,13 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>7</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" t="s">
-        <v>95</v>
-      </c>
-      <c r="H21" t="s">
-        <v>96</v>
-      </c>
-      <c r="I21" t="s">
-        <v>97</v>
+        <v>6</v>
+      </c>
+      <c r="D21" s="0">
+        <v>8</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1624,39 +1654,45 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>8</v>
-      </c>
-      <c r="D22">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="D22" s="0">
+        <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" t="s">
-        <v>99</v>
-      </c>
-      <c r="J22">
-        <v>2</v>
+        <v>70</v>
+      </c>
+      <c r="G22" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" t="s">
+        <v>96</v>
+      </c>
+      <c r="I22" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="D23" s="0">
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="F23" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1666,11 +1702,11 @@
       <c r="B24">
         <v>0</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
+      <c r="C24" s="0">
+        <v>0</v>
+      </c>
+      <c r="D24" s="0">
+        <v>2</v>
       </c>
       <c r="E24" t="s">
         <v>101</v>
@@ -1692,8 +1728,8 @@
       <c r="B25">
         <v>0</v>
       </c>
-      <c r="C25">
-        <v>2</v>
+      <c r="C25" s="0">
+        <v>1</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -1721,11 +1757,11 @@
       <c r="B26">
         <v>0</v>
       </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
+      <c r="C26" s="0">
+        <v>2</v>
+      </c>
+      <c r="D26" s="0">
+        <v>4</v>
       </c>
       <c r="E26" t="s">
         <v>108</v>
@@ -1747,11 +1783,11 @@
       <c r="B27">
         <v>0</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="0">
+        <v>3</v>
+      </c>
+      <c r="D27" s="0">
         <v>4</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
       </c>
       <c r="E27" t="s">
         <v>112</v>
@@ -1773,11 +1809,11 @@
       <c r="B28">
         <v>0</v>
       </c>
-      <c r="C28">
-        <v>5</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
+      <c r="C28" s="0">
+        <v>4</v>
+      </c>
+      <c r="D28" s="0">
+        <v>4</v>
       </c>
       <c r="E28" t="s">
         <v>116</v>
@@ -1799,8 +1835,8 @@
       <c r="B29">
         <v>0</v>
       </c>
-      <c r="C29">
-        <v>6</v>
+      <c r="C29" s="0">
+        <v>5</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -1828,11 +1864,11 @@
       <c r="B30">
         <v>0</v>
       </c>
-      <c r="C30">
-        <v>7</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
+      <c r="C30" s="0">
+        <v>6</v>
+      </c>
+      <c r="D30" s="0">
+        <v>2</v>
       </c>
       <c r="E30" t="s">
         <v>75</v>
@@ -1856,7 +1892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD447A5-A66D-423E-BEF4-4A4BB39A2411}">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1874,51 +1910,75 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>127</v>
+      <c r="A2" s="0">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>128</v>
+      <c r="A3" s="0">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="A4" s="0">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+      <c r="B5" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+      <c r="B6" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
+      <c r="B7" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>38</v>
+      <c r="B8" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated more of the pages and fixed the schrodinger's page bug
</commit_message>
<xml_diff>
--- a/app/src/main/assets/Book.xlsx
+++ b/app/src/main/assets/Book.xlsx
@@ -1119,7 +1119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC0EBA9-A7F4-428C-BDF6-604F23BD7DE8}">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="topLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1426,13 +1426,13 @@
       <c r="E12" t="s">
         <v>66</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>68</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" s="0" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a media player with resources for one instance and and updated database access classes, methods for the whole thing. Updated spread sheet and incremented db version
</commit_message>
<xml_diff>
--- a/app/src/main/assets/Book.xlsx
+++ b/app/src/main/assets/Book.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22918"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22920"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="442" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F8E40A43-5235-41A1-B759-66901D75D07E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2A335B4-BCE2-498D-9C73-C63850D12BFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="1" windowHeight="8010" windowWidth="14805" xWindow="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="105"/>
+    <workbookView activeTab="3" firstSheet="2" windowHeight="8010" windowWidth="14805" xWindow="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="105"/>
   </bookViews>
   <sheets>
     <sheet name="Module" sheetId="1" r:id="rId1"/>
     <sheet name="Lesson" sheetId="2" r:id="rId2"/>
     <sheet name="Page" sheetId="3" r:id="rId3"/>
-    <sheet name="PageType" sheetId="4" r:id="rId4"/>
-    <sheet name="Image" sheetId="5" r:id="rId5"/>
-    <sheet name="Activity" sheetId="6" r:id="rId6"/>
+    <sheet name="Media" sheetId="7" r:id="rId4"/>
+    <sheet name="PageType" sheetId="4" r:id="rId5"/>
+    <sheet name="Image" sheetId="5" r:id="rId6"/>
+    <sheet name="Activity" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="226">
   <si>
     <t>Number</t>
   </si>
@@ -149,6 +150,15 @@
     <t>Actiivty</t>
   </si>
   <si>
+    <t>Paypyrus</t>
+  </si>
+  <si>
+    <t>Tap anywhere to continue!</t>
+  </si>
+  <si>
+    <t>When we read we being with Alif, Baa', Taa'</t>
+  </si>
+  <si>
     <t>Read and Write Arabic Right</t>
   </si>
   <si>
@@ -332,9 +342,6 @@
     <t>You have unlocked Lesson 2 - The Keys to Written Arabic</t>
   </si>
   <si>
-    <t>When we read we being with Alif, Baa', Taa'</t>
-  </si>
-  <si>
     <t>Welcome to the First Letters Module</t>
   </si>
   <si>
@@ -410,22 +417,289 @@
     <t>You now have access to Module 3 - (To be or not to be) Connected</t>
   </si>
   <si>
+    <t>Page</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Content Page</t>
-  </si>
-  <si>
-    <t>Title Page</t>
-  </si>
-  <si>
-    <t>List Page</t>
-  </si>
-  <si>
-    <t>Image Page</t>
-  </si>
-  <si>
-    <t>Media Page</t>
+    <t>image</t>
+  </si>
+  <si>
+    <t>sound</t>
+  </si>
+  <si>
+    <t>alif</t>
+  </si>
+  <si>
+    <t>ic_letter_alif.xml</t>
+  </si>
+  <si>
+    <t>alif.wav</t>
+  </si>
+  <si>
+    <t>baa</t>
+  </si>
+  <si>
+    <t>ic_letter_baa.xml</t>
+  </si>
+  <si>
+    <t>baa.wav</t>
+  </si>
+  <si>
+    <t>taa</t>
+  </si>
+  <si>
+    <t>ic_letter_taa.xml</t>
+  </si>
+  <si>
+    <t>taa.wav</t>
+  </si>
+  <si>
+    <t>thaa</t>
+  </si>
+  <si>
+    <t>ic_letter_thaa.xml</t>
+  </si>
+  <si>
+    <t>thaa.wav</t>
+  </si>
+  <si>
+    <t>jeem</t>
+  </si>
+  <si>
+    <t>ic_letter_jeem.xml</t>
+  </si>
+  <si>
+    <t>Haa</t>
+  </si>
+  <si>
+    <t>ic_letter_hhaa.xml</t>
+  </si>
+  <si>
+    <t>hhaa.wav</t>
+  </si>
+  <si>
+    <t>khaa</t>
+  </si>
+  <si>
+    <t>ic_letter_khaa.xml</t>
+  </si>
+  <si>
+    <t>daal</t>
+  </si>
+  <si>
+    <t>ic_letter_daal.xml</t>
+  </si>
+  <si>
+    <t>daal.wav</t>
+  </si>
+  <si>
+    <t>dhaal</t>
+  </si>
+  <si>
+    <t>ic_letter_dhaalxml</t>
+  </si>
+  <si>
+    <t>dhaal.wav</t>
+  </si>
+  <si>
+    <t>raa</t>
+  </si>
+  <si>
+    <t>ic_letter_raa.xml</t>
+  </si>
+  <si>
+    <t>raa.wav</t>
+  </si>
+  <si>
+    <t>zaa</t>
+  </si>
+  <si>
+    <t>ic_letter_zaa.xml</t>
+  </si>
+  <si>
+    <t>zaa.wav</t>
+  </si>
+  <si>
+    <t>seen</t>
+  </si>
+  <si>
+    <t>ic_letter_seen.xml</t>
+  </si>
+  <si>
+    <t>seen.wav</t>
+  </si>
+  <si>
+    <t>sheen</t>
+  </si>
+  <si>
+    <t>ic_letter_sheen.xml</t>
+  </si>
+  <si>
+    <t>sheen.wav</t>
+  </si>
+  <si>
+    <t>saad</t>
+  </si>
+  <si>
+    <t>ic_letter_saad.xml</t>
+  </si>
+  <si>
+    <t>saad.wav</t>
+  </si>
+  <si>
+    <t>daad</t>
+  </si>
+  <si>
+    <t>ic_letter_daad.xml</t>
+  </si>
+  <si>
+    <t>daad.wav</t>
+  </si>
+  <si>
+    <t>Taa</t>
+  </si>
+  <si>
+    <t>ic_letter_ttaa.xml</t>
+  </si>
+  <si>
+    <t>ttaa.wav</t>
+  </si>
+  <si>
+    <t>dhaad</t>
+  </si>
+  <si>
+    <t>ic_letter_dhaad.xml</t>
+  </si>
+  <si>
+    <t>dhaad.wav</t>
+  </si>
+  <si>
+    <t>ayn</t>
+  </si>
+  <si>
+    <t>ic_letter_ayn.xml</t>
+  </si>
+  <si>
+    <t>ayn.wav</t>
+  </si>
+  <si>
+    <t>ghayn</t>
+  </si>
+  <si>
+    <t>ic_letter_ghayn.xml</t>
+  </si>
+  <si>
+    <t>ghayn.wav</t>
+  </si>
+  <si>
+    <t>faa</t>
+  </si>
+  <si>
+    <t>ic_letter_faa.xml</t>
+  </si>
+  <si>
+    <t>faa.wav</t>
+  </si>
+  <si>
+    <t>qaaf</t>
+  </si>
+  <si>
+    <t>ic_letter_qaaf.xml</t>
+  </si>
+  <si>
+    <t>qaaf.wav</t>
+  </si>
+  <si>
+    <t>kaaf</t>
+  </si>
+  <si>
+    <t>ic_letter_kaaf.xml</t>
+  </si>
+  <si>
+    <t>kaaf.wav</t>
+  </si>
+  <si>
+    <t>laam</t>
+  </si>
+  <si>
+    <t>ic_letter_laam.xml</t>
+  </si>
+  <si>
+    <t>laam.wav</t>
+  </si>
+  <si>
+    <t>meem</t>
+  </si>
+  <si>
+    <t>ic_letter_meem.xml</t>
+  </si>
+  <si>
+    <t>meem.wav</t>
+  </si>
+  <si>
+    <t>noon</t>
+  </si>
+  <si>
+    <t>ic_letter_noon.xml</t>
+  </si>
+  <si>
+    <t>noon.wav</t>
+  </si>
+  <si>
+    <t>haa</t>
+  </si>
+  <si>
+    <t>ic_letter_haa.xml</t>
+  </si>
+  <si>
+    <t>haa.wav</t>
+  </si>
+  <si>
+    <t>yaa</t>
+  </si>
+  <si>
+    <t>ic_letter_yaa.xml</t>
+  </si>
+  <si>
+    <t>yaa.wav</t>
+  </si>
+  <si>
+    <t>waaw</t>
+  </si>
+  <si>
+    <t>ic_letter_waaw.xml</t>
+  </si>
+  <si>
+    <t>waaw.wav</t>
+  </si>
+  <si>
+    <t>splash</t>
+  </si>
+  <si>
+    <t>moduleSelection</t>
+  </si>
+  <si>
+    <t>moduleContent</t>
+  </si>
+  <si>
+    <t>moduleList</t>
+  </si>
+  <si>
+    <t>lessonSelection</t>
+  </si>
+  <si>
+    <t>lessonContent</t>
+  </si>
+  <si>
+    <t>lessonImage</t>
+  </si>
+  <si>
+    <t>mediaPlayer</t>
+  </si>
+  <si>
+    <t>activity</t>
   </si>
   <si>
     <t>alphabet.svg</t>
@@ -437,61 +711,106 @@
     <t>PickUpDucks</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Paypyrus</t>
-  </si>
-  <si>
-    <t>Tap anywhere to continue!</t>
-  </si>
-  <si>
-    <t>Get started with the basics</t>
-  </si>
-  <si>
-    <t>Starting out right ( to left!!!) with these preparatory lessons to get you going in the right (left) direction!</t>
-  </si>
-  <si>
-    <t>Splash Screen</t>
-  </si>
-  <si>
-    <t>splash</t>
-  </si>
-  <si>
-    <t>moduleSelection</t>
-  </si>
-  <si>
-    <t>moduleContent</t>
-  </si>
-  <si>
-    <t>ModuleList</t>
-  </si>
-  <si>
-    <t>lessonSelection</t>
-  </si>
-  <si>
-    <t>moduleList</t>
-  </si>
-  <si>
-    <t>lessonContent</t>
-  </si>
-  <si>
-    <t>lessonImage</t>
-  </si>
-  <si>
-    <t>mediaPlayer</t>
-  </si>
-  <si>
-    <t>Activity</t>
-  </si>
-  <si>
-    <t>activity</t>
+    <t>hhaa</t>
+  </si>
+  <si>
+    <t>ttaa</t>
+  </si>
+  <si>
+    <t>ic_letter_alif</t>
+  </si>
+  <si>
+    <t>ic_letter_baa</t>
+  </si>
+  <si>
+    <t>ic_letter_taa</t>
+  </si>
+  <si>
+    <t>ic_letter_thaa</t>
+  </si>
+  <si>
+    <t>ic_letter_jeem</t>
+  </si>
+  <si>
+    <t>ic_letter_hhaa</t>
+  </si>
+  <si>
+    <t>ic_letter_khaa.xmli</t>
+  </si>
+  <si>
+    <t>ic_letter_khaa</t>
+  </si>
+  <si>
+    <t>ic_letter_daal</t>
+  </si>
+  <si>
+    <t>ic_letter_dhaal</t>
+  </si>
+  <si>
+    <t>ic_letter_raa</t>
+  </si>
+  <si>
+    <t>ic_letter_zaa</t>
+  </si>
+  <si>
+    <t>ic_letter_seen</t>
+  </si>
+  <si>
+    <t>ic_letter_sheen</t>
+  </si>
+  <si>
+    <t>ic_letter_saad.</t>
+  </si>
+  <si>
+    <t>ic_letter_saad</t>
+  </si>
+  <si>
+    <t>ic_letter_daad</t>
+  </si>
+  <si>
+    <t>ic_letter_ttaa</t>
+  </si>
+  <si>
+    <t>ic_letter_dhaad</t>
+  </si>
+  <si>
+    <t>ic_letter_ayn</t>
+  </si>
+  <si>
+    <t>ic_letter_ghayn</t>
+  </si>
+  <si>
+    <t>ic_letter_faa</t>
+  </si>
+  <si>
+    <t>ic_letter_qaaf</t>
+  </si>
+  <si>
+    <t>ic_letter_kaaf</t>
+  </si>
+  <si>
+    <t>ic_letter_laam</t>
+  </si>
+  <si>
+    <t>ic_letter_meem</t>
+  </si>
+  <si>
+    <t>ic_letter_noon</t>
+  </si>
+  <si>
+    <t>ic_letter_haa</t>
+  </si>
+  <si>
+    <t>ic_letter_yaa</t>
+  </si>
+  <si>
+    <t>ic_letter_waaw</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" count="8" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
@@ -502,10 +821,18 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <i/>
       <color rgb="FF000000"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -541,11 +868,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -978,7 +1307,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4601532C-3460-47AD-AB42-D440D6914B38}">
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView topLeftCell="B12" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1171,64 +1500,64 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>0</v>
-      </c>
-      <c r="B2" s="0">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0">
-        <v>0</v>
-      </c>
-      <c r="B3" s="0">
-        <v>0</v>
-      </c>
-      <c r="C3" s="0">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0">
-        <v>1</v>
-      </c>
-      <c r="E3" s="0" t="s">
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="0">
+    <row r="4" spans="1:11">
+      <c r="A4">
         <v>0</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>100</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1241,20 +1570,20 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" s="0">
+      <c r="D5">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1267,20 +1596,20 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="0">
+      <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1293,14 +1622,14 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7" s="0">
+      <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1310,23 +1639,23 @@
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" s="0">
-        <v>0</v>
-      </c>
-      <c r="D8" s="0">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H8" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1336,26 +1665,26 @@
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9" s="0">
-        <v>1</v>
-      </c>
-      <c r="D9" s="0">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1365,23 +1694,23 @@
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="C10" s="0">
+      <c r="C10">
         <v>2</v>
       </c>
-      <c r="D10" s="0">
+      <c r="D10">
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1391,23 +1720,23 @@
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="C11" s="0">
+      <c r="C11">
         <v>3</v>
       </c>
-      <c r="D11" s="0">
+      <c r="D11">
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I11" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1417,23 +1746,23 @@
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12" s="0">
-        <v>4</v>
-      </c>
-      <c r="D12" s="0">
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="G12" t="s">
+        <v>70</v>
       </c>
       <c r="H12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I12" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1443,26 +1772,26 @@
       <c r="B13">
         <v>0</v>
       </c>
-      <c r="C13" s="0">
+      <c r="C13">
         <v>5</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G13" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="I13" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1472,23 +1801,23 @@
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14" s="0">
+      <c r="C14">
         <v>6</v>
       </c>
-      <c r="D14" s="0">
+      <c r="D14">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1501,20 +1830,20 @@
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="D15" s="0">
+      <c r="D15">
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G15" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H15" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I15" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1527,14 +1856,14 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="0">
+      <c r="D16">
         <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F16" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1550,17 +1879,17 @@
       <c r="C17">
         <v>2</v>
       </c>
-      <c r="D17" s="0">
+      <c r="D17">
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G17" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H17" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1573,20 +1902,20 @@
       <c r="C18">
         <v>3</v>
       </c>
-      <c r="D18" s="0">
+      <c r="D18">
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G18" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H18" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="I18" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1599,11 +1928,11 @@
       <c r="C19">
         <v>4</v>
       </c>
-      <c r="D19" s="0">
+      <c r="D19">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1616,14 +1945,14 @@
       <c r="C20">
         <v>5</v>
       </c>
-      <c r="D20" s="0">
+      <c r="D20">
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F20" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -1639,7 +1968,7 @@
       <c r="C21">
         <v>6</v>
       </c>
-      <c r="D21" s="0">
+      <c r="D21">
         <v>8</v>
       </c>
       <c r="K21">
@@ -1656,20 +1985,20 @@
       <c r="C22">
         <v>7</v>
       </c>
-      <c r="D22" s="0">
+      <c r="D22">
         <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G22" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H22" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="I22" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1682,14 +2011,14 @@
       <c r="C23">
         <v>8</v>
       </c>
-      <c r="D23" s="0">
+      <c r="D23">
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F23" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="J23">
         <v>2</v>
@@ -1702,23 +2031,23 @@
       <c r="B24">
         <v>0</v>
       </c>
-      <c r="C24" s="0">
-        <v>0</v>
-      </c>
-      <c r="D24" s="0">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G24" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H24" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1728,26 +2057,26 @@
       <c r="B25">
         <v>0</v>
       </c>
-      <c r="C25" s="0">
+      <c r="C25">
         <v>1</v>
       </c>
       <c r="D25">
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G25" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H25" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I25" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1757,23 +2086,23 @@
       <c r="B26">
         <v>0</v>
       </c>
-      <c r="C26" s="0">
+      <c r="C26">
         <v>2</v>
       </c>
-      <c r="D26" s="0">
+      <c r="D26">
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G26" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I26" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1783,23 +2112,23 @@
       <c r="B27">
         <v>0</v>
       </c>
-      <c r="C27" s="0">
+      <c r="C27">
         <v>3</v>
       </c>
-      <c r="D27" s="0">
+      <c r="D27">
         <v>4</v>
       </c>
       <c r="E27" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G27" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I27" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1809,23 +2138,23 @@
       <c r="B28">
         <v>0</v>
       </c>
-      <c r="C28" s="0">
-        <v>4</v>
-      </c>
-      <c r="D28" s="0">
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
         <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G28" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H28" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I28" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1835,26 +2164,26 @@
       <c r="B29">
         <v>0</v>
       </c>
-      <c r="C29" s="0">
+      <c r="C29">
         <v>5</v>
       </c>
       <c r="D29">
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F29" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G29" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H29" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I29" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1864,23 +2193,23 @@
       <c r="B30">
         <v>0</v>
       </c>
-      <c r="C30" s="0">
+      <c r="C30">
         <v>6</v>
       </c>
-      <c r="D30" s="0">
+      <c r="D30">
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G30" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H30" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I30" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1889,6 +2218,692 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D250514-EA63-493A-80CA-497BF9C33864}">
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0" tabSelected="1">
+      <selection pane="topLeft" activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.57" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>154</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>163</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>166</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>169</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>172</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>178</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>17</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>184</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>187</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>190</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>193</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>22</v>
+      </c>
+      <c r="E24" t="s">
+        <v>196</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>23</v>
+      </c>
+      <c r="E25" t="s">
+        <v>199</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>202</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>25</v>
+      </c>
+      <c r="E27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>208</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>27</v>
+      </c>
+      <c r="E29" t="s">
+        <v>211</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD447A5-A66D-423E-BEF4-4A4BB39A2411}">
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1906,79 +2921,79 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="0">
-        <v>0</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>141</v>
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="0">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>142</v>
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>143</v>
+      <c r="B4" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>146</v>
+      <c r="B5" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="0">
-        <v>4</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>145</v>
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0">
+      <c r="B7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0">
+      <c r="B8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0">
+      <c r="B9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>151</v>
+      <c r="B10" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -1986,7 +3001,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30587C1B-3062-4125-8D73-822059D87865}">
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2003,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2011,7 +3026,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2019,7 +3034,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -2027,7 +3042,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996951D6-D811-4EA7-B062-C55A0ACDC35A}">
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2044,7 +3059,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>